<commit_message>
Fehler im Übersicht-Sheet gefixt, aufgeräumt
</commit_message>
<xml_diff>
--- a/Tagestimer.xlsx
+++ b/Tagestimer.xlsx
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
   <si>
     <t>Stunden</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Erg</t>
   </si>
   <si>
-    <t>MigStufe4</t>
-  </si>
-  <si>
     <t>Compatibility Report for 2011 KW 44 Tagestimer.xls</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
   </si>
   <si>
     <t>konto10</t>
-  </si>
-  <si>
-    <t>konto11</t>
   </si>
   <si>
     <t>Richtig was geschafft</t>
@@ -710,7 +704,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -888,12 +882,41 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1183,7 +1206,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.4274711168164313"/>
-          <c:y val="2.7777777777777964E-2"/>
+          <c:y val="2.7777777777777981E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1216,7 +1239,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.27727856225930803"/>
+          <c:x val="0.27727856225930814"/>
           <c:y val="0.2021607984917512"/>
           <c:w val="0.44672657252888331"/>
           <c:h val="0.53703784637503371"/>
@@ -1548,9 +1571,6 @@
               <c:f>Übersicht!$B$3:$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>MigStufe4</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>einkaufen</c:v>
                 </c:pt>
@@ -1582,7 +1602,7 @@
                   <c:v>konto10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>konto11</c:v>
+                  <c:v>.</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>.</c:v>
@@ -1639,6 +1659,9 @@
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -1785,7 +1808,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000089" footer="0.49212598450000089"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598450000095" footer="0.49212598450000095"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2160,10 +2183,10 @@
         <v>0.125</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -2178,19 +2201,19 @@
         <v>0.20833333333333337</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="2">
-        <f t="shared" ref="B4:B9" si="1">C4</f>
+        <f t="shared" ref="B5:B9" si="1">C4</f>
         <v>0.75</v>
       </c>
       <c r="C5" s="29">
-        <f t="shared" ref="C3:C9" si="2">B5</f>
+        <f t="shared" ref="C5:C9" si="2">B5</f>
         <v>0.75</v>
       </c>
       <c r="D5" s="23">
@@ -2581,7 +2604,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>Übersicht!B14</f>
-        <v>konto11</v>
+        <v>.</v>
       </c>
       <c r="E33" s="28" t="str">
         <f t="shared" si="6"/>
@@ -2788,25 +2811,25 @@
   <autoFilter ref="B2:F19"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="37" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C47 D3:D15">
-    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="34" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="5" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2833,7 +2856,7 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="43"/>
       <c r="D1" s="51"/>
@@ -2841,7 +2864,7 @@
     </row>
     <row r="2" spans="2:5">
       <c r="B2" s="59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="51"/>
@@ -2855,7 +2878,7 @@
     </row>
     <row r="4" spans="2:5" ht="38.25">
       <c r="B4" s="60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="52"/>
@@ -2869,12 +2892,12 @@
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="51"/>
       <c r="E6" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="13.5" thickBot="1">
@@ -2885,7 +2908,7 @@
     </row>
     <row r="8" spans="2:5" ht="51">
       <c r="B8" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="54"/>
@@ -2898,7 +2921,7 @@
       <c r="C9" s="44"/>
       <c r="D9" s="52"/>
       <c r="E9" s="63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="26.25" thickBot="1">
@@ -2906,7 +2929,7 @@
       <c r="C10" s="50"/>
       <c r="D10" s="57"/>
       <c r="E10" s="64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -3390,7 +3413,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>Übersicht!B14</f>
-        <v>konto11</v>
+        <v>.</v>
       </c>
       <c r="E33" s="28" t="str">
         <f t="shared" si="4"/>
@@ -3597,25 +3620,25 @@
   <autoFilter ref="B2:F19"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="cellIs" dxfId="31" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="30" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C47 D3:D15">
-    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4102,7 +4125,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>Übersicht!B14</f>
-        <v>konto11</v>
+        <v>.</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="4"/>
@@ -4309,25 +4332,25 @@
   <autoFilter ref="B2:F19"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="cellIs" dxfId="26" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C47 D3:D15">
-    <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4799,7 +4822,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>Übersicht!B14</f>
-        <v>konto11</v>
+        <v>.</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5006,25 +5029,25 @@
   <autoFilter ref="B2:F19"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C47 D3:D15">
-    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5513,7 +5536,7 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>Übersicht!B14</f>
-        <v>konto11</v>
+        <v>.</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="4"/>
@@ -5720,25 +5743,25 @@
   <autoFilter ref="B2:F20"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16 C23:C47">
-    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B16">
-    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C16">
-    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5765,7 +5788,7 @@
     <col min="2" max="2" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="11.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="6.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="1.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="71.85546875" style="39" customWidth="1"/>
@@ -5778,10 +5801,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="106" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="20.100000000000001" customHeight="1">
@@ -5814,15 +5837,13 @@
       <c r="M2" s="104"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="75"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="75"/>
       <c r="E3" s="75"/>
       <c r="F3" s="75"/>
       <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="75"/>
       <c r="J3" s="76"/>
       <c r="L3" s="65" t="s">
@@ -5834,7 +5855,7 @@
     </row>
     <row r="4" spans="2:14" ht="12.75" customHeight="1">
       <c r="B4" s="69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B4,Montag!$D$3:$D$15)</f>
@@ -5876,7 +5897,7 @@
     </row>
     <row r="5" spans="2:14" ht="12.75" customHeight="1">
       <c r="B5" s="69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B5,Montag!$D$3:$D$15)</f>
@@ -5918,7 +5939,7 @@
     </row>
     <row r="6" spans="2:14" ht="12.75" customHeight="1">
       <c r="B6" s="69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B6,Montag!$D$3:$D$15)</f>
@@ -5960,7 +5981,7 @@
     </row>
     <row r="7" spans="2:14" ht="12.75" customHeight="1">
       <c r="B7" s="69" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B7,Montag!$D$3:$D$15)</f>
@@ -6002,14 +6023,32 @@
     </row>
     <row r="8" spans="2:14" ht="12.75" customHeight="1">
       <c r="B8" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="95"/>
+        <v>39</v>
+      </c>
+      <c r="C8" s="95">
+        <f>SUMIF(Montag!$F$3:$F$15, $B8,Montag!$D$3:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="95">
+        <f>SUMIF(Dienstag!$F$3:$F$15, $B8,Dienstag!$D$3:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="95">
+        <f>SUMIF(Mittwoch!$F$3:$F$15, $B8,Mittwoch!$D$3:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="95">
+        <f>SUMIF(Donnerstag!$F$3:$F$15, $B8,Donnerstag!$D$3:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="95">
+        <f>SUMIF(Freitag!$F$3:$F$16, $B8,Freitag!$D$3:$D$16)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="95">
+        <f t="shared" ref="H8:H11" si="2">SUM(C8:G8)</f>
+        <v>0</v>
+      </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="L8" s="95" t="str">
@@ -6026,30 +6065,30 @@
     </row>
     <row r="9" spans="2:14" ht="12.75" customHeight="1">
       <c r="B9" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="19">
+        <v>40</v>
+      </c>
+      <c r="C9" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B9,Montag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="95">
         <f>SUMIF(Dienstag!$F$3:$F$15, $B9,Dienstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="95">
         <f>SUMIF(Mittwoch!$F$3:$F$15, $B9,Mittwoch!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="95">
         <f>SUMIF(Donnerstag!$F$3:$F$15, $B9,Donnerstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="95">
         <f>SUMIF(Freitag!$F$3:$F$16, $B9,Freitag!$D$3:$D$16)</f>
         <v>0</v>
       </c>
       <c r="H9" s="95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I9" s="21"/>
@@ -6068,30 +6107,30 @@
     </row>
     <row r="10" spans="2:14" ht="12.75" customHeight="1">
       <c r="B10" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="19">
+        <v>41</v>
+      </c>
+      <c r="C10" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B10,Montag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="95">
         <f>SUMIF(Dienstag!$F$3:$F$15, $B10,Dienstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="95">
         <f>SUMIF(Mittwoch!$F$3:$F$15, $B10,Mittwoch!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="95">
         <f>SUMIF(Donnerstag!$F$3:$F$15, $B10,Donnerstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="95">
         <f>SUMIF(Freitag!$F$3:$F$16, $B10,Freitag!$D$3:$D$16)</f>
         <v>0</v>
       </c>
       <c r="H10" s="95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10" s="21"/>
@@ -6110,30 +6149,30 @@
     </row>
     <row r="11" spans="2:14" ht="12.75" customHeight="1">
       <c r="B11" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="19">
+        <v>42</v>
+      </c>
+      <c r="C11" s="95">
         <f>SUMIF(Montag!$F$3:$F$15, $B11,Montag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="95">
         <f>SUMIF(Dienstag!$F$3:$F$15, $B11,Dienstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="95">
         <f>SUMIF(Mittwoch!$F$3:$F$15, $B11,Mittwoch!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="95">
         <f>SUMIF(Donnerstag!$F$3:$F$15, $B11,Donnerstag!$D$3:$D$15)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="95">
         <f>SUMIF(Freitag!$F$3:$F$16, $B11,Freitag!$D$3:$D$16)</f>
         <v>0</v>
       </c>
       <c r="H11" s="95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11" s="21"/>
@@ -6152,7 +6191,7 @@
     </row>
     <row r="12" spans="2:14" ht="12.75" customHeight="1">
       <c r="B12" s="69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B12,Montag!$D$3:$D$15)</f>
@@ -6191,7 +6230,7 @@
     </row>
     <row r="13" spans="2:14" ht="12.75" customHeight="1">
       <c r="B13" s="69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B13,Montag!$D$3:$D$15)</f>
@@ -6214,13 +6253,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="95">
-        <f t="shared" ref="H13:H19" si="2">SUM(C13:G13)</f>
+        <f t="shared" ref="H13:H19" si="3">SUM(C13:G13)</f>
         <v>0</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
       <c r="L13" s="95" t="str">
-        <f t="shared" ref="L13:L22" si="3">B13</f>
+        <f t="shared" ref="L13:L22" si="4">B13</f>
         <v>konto10</v>
       </c>
       <c r="M13" s="40" t="str">
@@ -6230,7 +6269,7 @@
     </row>
     <row r="14" spans="2:14" ht="12.75" customHeight="1">
       <c r="B14" s="69" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C14" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B14,Montag!$D$3:$D$15)</f>
@@ -6253,14 +6292,14 @@
         <v>0</v>
       </c>
       <c r="H14" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
       <c r="L14" s="95" t="str">
-        <f t="shared" si="3"/>
-        <v>konto11</v>
+        <f t="shared" si="4"/>
+        <v>.</v>
       </c>
       <c r="M14" s="40" t="str">
         <f>IF(C14&gt;0,"[Mo] "&amp;Montag!E33,"")&amp;IF(D14&gt;0," [Di] "&amp;Dienstag!E33,"")&amp;IF(E14&gt;0," [Mi] "&amp;Mittwoch!E33,"")&amp;IF(F14&gt;0," [Do] "&amp;Donnerstag!E33,"")&amp;IF(G14&gt;0," [Fr] "&amp;Freitag!E33,"")</f>
@@ -6269,7 +6308,7 @@
     </row>
     <row r="15" spans="2:14" ht="12.75" customHeight="1">
       <c r="B15" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B15,Montag!$D$3:$D$15)</f>
@@ -6292,13 +6331,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="L15" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M15" s="40" t="str">
@@ -6308,7 +6347,7 @@
     </row>
     <row r="16" spans="2:14" ht="12.75" customHeight="1">
       <c r="B16" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B16,Montag!$D$3:$D$15)</f>
@@ -6331,13 +6370,13 @@
         <v>0</v>
       </c>
       <c r="H16" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="L16" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M16" s="40" t="str">
@@ -6347,7 +6386,7 @@
     </row>
     <row r="17" spans="2:14" ht="12.75" customHeight="1">
       <c r="B17" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B17,Montag!$D$3:$D$15)</f>
@@ -6370,13 +6409,13 @@
         <v>0</v>
       </c>
       <c r="H17" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="L17" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M17" s="40" t="str">
@@ -6389,7 +6428,7 @@
     </row>
     <row r="18" spans="2:14" ht="12.75" customHeight="1">
       <c r="B18" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B18,Montag!$D$3:$D$15)</f>
@@ -6412,13 +6451,13 @@
         <v>0</v>
       </c>
       <c r="H18" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
       <c r="L18" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M18" s="40" t="str">
@@ -6431,7 +6470,7 @@
     </row>
     <row r="19" spans="2:14" ht="12.75" customHeight="1">
       <c r="B19" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B19,Montag!$D$3:$D$15)</f>
@@ -6454,13 +6493,13 @@
         <v>0</v>
       </c>
       <c r="H19" s="95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
       <c r="L19" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M19" s="40" t="str">
@@ -6473,7 +6512,7 @@
     </row>
     <row r="20" spans="2:14" ht="12.75" customHeight="1">
       <c r="B20" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B20,Montag!$D$3:$D$15)</f>
@@ -6496,13 +6535,13 @@
         <v>0</v>
       </c>
       <c r="H20" s="95">
-        <f t="shared" ref="H20:H26" si="4">SUM(C20:G20)</f>
+        <f t="shared" ref="H20:H26" si="5">SUM(C20:G20)</f>
         <v>0</v>
       </c>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
       <c r="L20" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M20" s="40" t="str">
@@ -6515,7 +6554,7 @@
     </row>
     <row r="21" spans="2:14" ht="12.75" customHeight="1">
       <c r="B21" s="105" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B21,Montag!$D$3:$D$15)</f>
@@ -6538,13 +6577,13 @@
         <v>0</v>
       </c>
       <c r="H21" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="L21" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M21" s="40" t="str">
@@ -6554,7 +6593,7 @@
     </row>
     <row r="22" spans="2:14" ht="12.75" customHeight="1">
       <c r="B22" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B22,Montag!$D$3:$D$15)</f>
@@ -6577,13 +6616,13 @@
         <v>0</v>
       </c>
       <c r="H22" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
       <c r="L22" s="95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="M22" s="40" t="str">
@@ -6596,7 +6635,7 @@
     </row>
     <row r="23" spans="2:14" ht="12.75" customHeight="1">
       <c r="B23" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B23,Montag!$D$3:$D$15)</f>
@@ -6619,7 +6658,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I23" s="21"/>
@@ -6638,7 +6677,7 @@
     </row>
     <row r="24" spans="2:14" ht="12.75" customHeight="1">
       <c r="B24" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B24,Montag!$D$3:$D$15)</f>
@@ -6661,7 +6700,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I24" s="21"/>
@@ -6680,7 +6719,7 @@
     </row>
     <row r="25" spans="2:14" ht="12.75" customHeight="1">
       <c r="B25" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B25,Montag!$D$3:$D$15)</f>
@@ -6703,7 +6742,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="95">
-        <f t="shared" ref="H25" si="5">SUM(C25:G25)</f>
+        <f t="shared" ref="H25" si="6">SUM(C25:G25)</f>
         <v>0</v>
       </c>
       <c r="I25" s="21"/>
@@ -6722,7 +6761,7 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="19">
         <f>SUMIF(Montag!$F$3:$F$15, $B26,Montag!$D$3:$D$15)</f>
@@ -6745,7 +6784,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I26" s="21"/>
@@ -6886,55 +6925,55 @@
   <autoFilter ref="L3:L12"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C28:G28">
-    <cfRule type="cellIs" dxfId="12" priority="18" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>C$27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="11" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:J11 L4:L25 C4:H24 C26:H26 H8:H25">
-    <cfRule type="cellIs" dxfId="10" priority="20" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C11:J11 L4:L25 C26:H26 H8:H25 C4:H24">
+    <cfRule type="cellIs" dxfId="14" priority="20" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:G25 I25:J25">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:J11 L4:L25 C26:H26 C4:H10 C12:H24 H8:H25">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C11:J11 L4:L25 C26:H26 H8:H25 C4:H24">
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:G25 I25:J25">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7139,12 +7178,12 @@
   <autoFilter ref="B2:F16"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C15">
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
       <formula>B4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7203,7 +7242,7 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="43"/>
       <c r="D1" s="51"/>
@@ -7211,7 +7250,7 @@
     </row>
     <row r="2" spans="2:5">
       <c r="B2" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="51"/>
@@ -7225,7 +7264,7 @@
     </row>
     <row r="4" spans="2:5" ht="38.25">
       <c r="B4" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="52"/>
@@ -7239,12 +7278,12 @@
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="51"/>
       <c r="E6" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="13.5" thickBot="1">
@@ -7255,7 +7294,7 @@
     </row>
     <row r="8" spans="2:5" ht="51">
       <c r="B8" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="54"/>
@@ -7268,7 +7307,7 @@
       <c r="C9" s="44"/>
       <c r="D9" s="52"/>
       <c r="E9" s="56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="26.25" thickBot="1">
@@ -7276,7 +7315,7 @@
       <c r="C10" s="50"/>
       <c r="D10" s="57"/>
       <c r="E10" s="58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:5">

</xml_diff>